<commit_message>
add import functionality for product problems in returned products
</commit_message>
<xml_diff>
--- a/public/assets/excel-templates/imports/aftersales/product-problem-import.xlsx
+++ b/public/assets/excel-templates/imports/aftersales/product-problem-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\rekachain-web\public\assets\excel-templates\imports\aftersales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427F4F16-74D0-4C77-8B10-4DEF55D0BABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A535170-5B8F-440F-A685-551E47D85277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2220" windowWidth="21600" windowHeight="11835" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
+    <workbookView xWindow="7590" yWindow="7680" windowWidth="21600" windowHeight="11835" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Produk" sheetId="2" r:id="rId1"/>
@@ -36,12 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Komponen Bermasalah</t>
-  </si>
-  <si>
-    <t>Penanganan</t>
-  </si>
-  <si>
     <t>Diganti</t>
   </si>
   <si>
@@ -51,9 +45,6 @@
     <t>Light</t>
   </si>
   <si>
-    <t>Keterangan</t>
-  </si>
-  <si>
     <t>Tidak Terang</t>
   </si>
   <si>
@@ -61,6 +52,15 @@
   </si>
   <si>
     <t>Lepas</t>
+  </si>
+  <si>
+    <t>Problem Component Name</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -139,9 +139,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="2" xr3:uid="{B4B3E70E-BACA-47F7-9D7C-35164148A046}" name="Komponen Bermasalah"/>
-    <tableColumn id="1" xr3:uid="{CA71D7E8-0596-4F88-975E-B4F82B5B3899}" name="Keterangan"/>
-    <tableColumn id="3" xr3:uid="{2DA4E1DE-BBC8-4C19-8C43-2AB785A23093}" name="Penanganan"/>
+    <tableColumn id="2" xr3:uid="{B4B3E70E-BACA-47F7-9D7C-35164148A046}" name="Problem Component Name"/>
+    <tableColumn id="1" xr3:uid="{CA71D7E8-0596-4F88-975E-B4F82B5B3899}" name="Note"/>
+    <tableColumn id="3" xr3:uid="{2DA4E1DE-BBC8-4C19-8C43-2AB785A23093}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -448,7 +448,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,35 +459,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>